<commit_message>
Fix quantities on 2WLS-30W-BOM
</commit_message>
<xml_diff>
--- a/2WLS-30W-BOM.xlsx
+++ b/2WLS-30W-BOM.xlsx
@@ -127,15 +127,9 @@
     <t>C1, C2, C4, C5</t>
   </si>
   <si>
-    <t>C7, C8</t>
-  </si>
-  <si>
     <t>L1, L2</t>
   </si>
   <si>
-    <t>5V DCDC Converter (see also Recom/Delta alternates on PCB)</t>
-  </si>
-  <si>
     <t>EC6C06</t>
   </si>
   <si>
@@ -145,7 +139,13 @@
     <t>U2</t>
   </si>
   <si>
-    <t>15V DCDC Dual Converter (see also Recom/Delta alternates on PCB)</t>
+    <t xml:space="preserve">15V DCDC Dual Converter </t>
+  </si>
+  <si>
+    <t>5V DCDC Converter</t>
+  </si>
+  <si>
+    <t>C7, C8,C9</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,7 +517,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -551,7 +551,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -559,13 +559,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -588,7 +588,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -599,22 +599,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>